<commit_message>
Test for generation data service model complet
</commit_message>
<xml_diff>
--- a/lib/assets/20151030_Existing_generating_plant.xlsx
+++ b/lib/assets/20151030_Existing_generating_plant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevetorrens/workspace-ror/ghgemissions/lib/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028CB241-EBF2-C14C-A2AA-F6481008ACDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8431F18C-62C1-6A43-9ABE-CCF73846350E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generating Stations" sheetId="1" r:id="rId1"/>
@@ -4390,16 +4390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AB226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4520,7 +4520,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:28" hidden="1">
+    <row r="2" spans="1:28">
       <c r="A2" s="2" t="s">
         <v>326</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="3" spans="1:28" hidden="1">
+    <row r="3" spans="1:28">
       <c r="A3" s="2" t="s">
         <v>342</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="4" spans="1:28" hidden="1">
+    <row r="4" spans="1:28">
       <c r="A4" s="2" t="s">
         <v>1175</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1">
+    <row r="5" spans="1:28">
       <c r="A5" s="2" t="s">
         <v>346</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:28" hidden="1">
+    <row r="6" spans="1:28">
       <c r="A6" s="2" t="s">
         <v>353</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:28" hidden="1">
+    <row r="7" spans="1:28">
       <c r="A7" s="2" t="s">
         <v>363</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:28" hidden="1">
+    <row r="8" spans="1:28">
       <c r="A8" s="2" t="s">
         <v>922</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="9" spans="1:28" hidden="1">
+    <row r="9" spans="1:28">
       <c r="A9" s="2" t="s">
         <v>926</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="10" spans="1:28" hidden="1">
+    <row r="10" spans="1:28">
       <c r="A10" s="2" t="s">
         <v>934</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:28" hidden="1">
+    <row r="11" spans="1:28">
       <c r="A11" s="3" t="s">
         <v>612</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="12" spans="1:28" hidden="1">
+    <row r="12" spans="1:28">
       <c r="A12" s="2" t="s">
         <v>940</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:28" hidden="1">
+    <row r="14" spans="1:28">
       <c r="A14" s="2" t="s">
         <v>952</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:28" hidden="1">
+    <row r="15" spans="1:28">
       <c r="A15" s="2" t="s">
         <v>960</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:28" hidden="1">
+    <row r="17" spans="1:28">
       <c r="A17" s="3" t="s">
         <v>188</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1">
+    <row r="18" spans="1:28">
       <c r="A18" s="2" t="s">
         <v>970</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:28" hidden="1">
+    <row r="19" spans="1:28">
       <c r="A19" s="2" t="s">
         <v>974</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1">
+    <row r="20" spans="1:28">
       <c r="A20" s="2" t="s">
         <v>754</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="21" spans="1:28" hidden="1">
+    <row r="21" spans="1:28">
       <c r="A21" s="2" t="s">
         <v>980</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="22" spans="1:28" hidden="1">
+    <row r="22" spans="1:28">
       <c r="A22" s="2" t="s">
         <v>985</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1">
+    <row r="23" spans="1:28">
       <c r="A23" s="3" t="s">
         <v>862</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:28" hidden="1">
+    <row r="24" spans="1:28">
       <c r="A24" s="2" t="s">
         <v>990</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1">
+    <row r="25" spans="1:28">
       <c r="A25" s="2" t="s">
         <v>995</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="26" spans="1:28" hidden="1">
+    <row r="26" spans="1:28">
       <c r="A26" s="2" t="s">
         <v>1001</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="27" spans="1:28" hidden="1">
+    <row r="27" spans="1:28">
       <c r="A27" s="3" t="s">
         <v>1006</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="28" spans="1:28" hidden="1">
+    <row r="28" spans="1:28">
       <c r="A28" s="3" t="s">
         <v>872</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="13" hidden="1" customHeight="1">
+    <row r="29" spans="1:28" ht="13" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>599</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1">
+    <row r="30" spans="1:28">
       <c r="A30" s="2" t="s">
         <v>1010</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1">
+    <row r="31" spans="1:28">
       <c r="A31" s="2" t="s">
         <v>1016</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:28" hidden="1">
+    <row r="32" spans="1:28">
       <c r="A32" s="2" t="s">
         <v>1025</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:28" hidden="1">
+    <row r="33" spans="1:28">
       <c r="A33" s="2" t="s">
         <v>1030</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="35" spans="1:28" hidden="1">
+    <row r="35" spans="1:28">
       <c r="A35" s="3" t="s">
         <v>510</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:28" hidden="1">
+    <row r="36" spans="1:28">
       <c r="A36" s="2" t="s">
         <v>1036</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:28" hidden="1">
+    <row r="37" spans="1:28">
       <c r="A37" s="2" t="s">
         <v>1041</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:28" hidden="1">
+    <row r="38" spans="1:28">
       <c r="A38" s="2" t="s">
         <v>1045</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:28" hidden="1">
+    <row r="39" spans="1:28">
       <c r="A39" s="3" t="s">
         <v>831</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:28" hidden="1">
+    <row r="40" spans="1:28">
       <c r="A40" s="3" t="s">
         <v>1191</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:28" hidden="1">
+    <row r="41" spans="1:28">
       <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="34" customFormat="1" hidden="1">
+    <row r="42" spans="1:28" s="34" customFormat="1">
       <c r="A42" s="29" t="s">
         <v>1216</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:28" hidden="1">
+    <row r="43" spans="1:28">
       <c r="A43" s="2" t="s">
         <v>1049</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:28" hidden="1">
+    <row r="44" spans="1:28">
       <c r="A44" s="2" t="s">
         <v>760</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="46" spans="1:28" hidden="1">
+    <row r="46" spans="1:28">
       <c r="A46" s="2" t="s">
         <v>1051</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:28" hidden="1">
+    <row r="47" spans="1:28">
       <c r="A47" s="2" t="s">
         <v>1053</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:28" hidden="1">
+    <row r="48" spans="1:28">
       <c r="A48" s="2" t="s">
         <v>1058</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="1:28" hidden="1">
+    <row r="51" spans="1:28">
       <c r="A51" s="2" t="s">
         <v>1070</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:28" hidden="1">
+    <row r="52" spans="1:28">
       <c r="A52" s="3" t="s">
         <v>885</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:28" hidden="1">
+    <row r="53" spans="1:28">
       <c r="A53" s="2" t="s">
         <v>1076</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:28" hidden="1">
+    <row r="54" spans="1:28">
       <c r="A54" s="2" t="s">
         <v>43</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:28" hidden="1">
+    <row r="55" spans="1:28">
       <c r="A55" s="2" t="s">
         <v>49</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:28" hidden="1">
+    <row r="56" spans="1:28">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:28" hidden="1">
+    <row r="57" spans="1:28">
       <c r="A57" s="2" t="s">
         <v>63</v>
       </c>
@@ -9012,7 +9012,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="59" spans="1:28" hidden="1">
+    <row r="59" spans="1:28">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="60" spans="1:28" hidden="1">
+    <row r="60" spans="1:28">
       <c r="A60" s="3" t="s">
         <v>895</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:28" hidden="1">
+    <row r="61" spans="1:28">
       <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
@@ -9246,7 +9246,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="62" spans="1:28" hidden="1">
+    <row r="62" spans="1:28">
       <c r="A62" s="3" t="s">
         <v>875</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="67" spans="1:28" hidden="1">
+    <row r="67" spans="1:28">
       <c r="A67" s="2" t="s">
         <v>93</v>
       </c>
@@ -9792,7 +9792,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="69" spans="1:28" hidden="1">
+    <row r="69" spans="1:28">
       <c r="A69" s="2" t="s">
         <v>94</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="70" spans="1:28" hidden="1">
+    <row r="70" spans="1:28">
       <c r="A70" s="2" t="s">
         <v>98</v>
       </c>
@@ -9958,7 +9958,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:28" hidden="1">
+    <row r="71" spans="1:28">
       <c r="A71" s="2" t="s">
         <v>126</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="73" spans="1:28" hidden="1">
+    <row r="73" spans="1:28">
       <c r="A73" s="2" t="s">
         <v>137</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:28" hidden="1">
+    <row r="75" spans="1:28">
       <c r="A75" s="3" t="s">
         <v>662</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:28" hidden="1">
+    <row r="80" spans="1:28">
       <c r="A80" s="2" t="s">
         <v>249</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:28" hidden="1">
+    <row r="81" spans="1:28">
       <c r="A81" s="2" t="s">
         <v>252</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:28" hidden="1">
+    <row r="83" spans="1:28">
       <c r="A83" s="3" t="s">
         <v>800</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="84" spans="1:28" hidden="1">
+    <row r="84" spans="1:28">
       <c r="A84" s="2" t="s">
         <v>296</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:28" hidden="1">
+    <row r="85" spans="1:28">
       <c r="A85" s="3" t="s">
         <v>881</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:28" hidden="1">
+    <row r="86" spans="1:28">
       <c r="A86" s="2" t="s">
         <v>481</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="87" spans="1:28" hidden="1">
+    <row r="87" spans="1:28">
       <c r="A87" s="2" t="s">
         <v>482</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="34" customFormat="1" hidden="1">
+    <row r="88" spans="1:28" s="34" customFormat="1">
       <c r="A88" s="29" t="s">
         <v>1217</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:28" hidden="1">
+    <row r="89" spans="1:28">
       <c r="A89" s="2" t="s">
         <v>489</v>
       </c>
@@ -11456,7 +11456,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="90" spans="1:28" hidden="1">
+    <row r="90" spans="1:28">
       <c r="A90" s="2" t="s">
         <v>492</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="91" spans="1:28" hidden="1">
+    <row r="91" spans="1:28">
       <c r="A91" s="3" t="s">
         <v>901</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:28" hidden="1">
+    <row r="92" spans="1:28">
       <c r="A92" s="3" t="s">
         <v>269</v>
       </c>
@@ -11692,7 +11692,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="93" spans="1:28" hidden="1">
+    <row r="93" spans="1:28">
       <c r="A93" s="2" t="s">
         <v>495</v>
       </c>
@@ -11772,7 +11772,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:28" hidden="1">
+    <row r="94" spans="1:28">
       <c r="A94" s="2" t="s">
         <v>501</v>
       </c>
@@ -11926,7 +11926,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:28" hidden="1">
+    <row r="96" spans="1:28">
       <c r="A96" s="2" t="s">
         <v>506</v>
       </c>
@@ -12006,7 +12006,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="97" spans="1:28" hidden="1">
+    <row r="97" spans="1:28">
       <c r="A97" s="2" t="s">
         <v>508</v>
       </c>
@@ -12084,7 +12084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:28" hidden="1">
+    <row r="98" spans="1:28">
       <c r="A98" s="2" t="s">
         <v>513</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="1:28" hidden="1">
+    <row r="99" spans="1:28">
       <c r="A99" s="2" t="s">
         <v>515</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:28" hidden="1">
+    <row r="100" spans="1:28">
       <c r="A100" s="2" t="s">
         <v>519</v>
       </c>
@@ -12322,7 +12322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:28" hidden="1">
+    <row r="101" spans="1:28">
       <c r="A101" s="2" t="s">
         <v>521</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="102" spans="1:28" hidden="1">
+    <row r="102" spans="1:28">
       <c r="A102" s="2" t="s">
         <v>58</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="105" spans="1:28" hidden="1">
+    <row r="105" spans="1:28">
       <c r="A105" s="2" t="s">
         <v>531</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:28" hidden="1">
+    <row r="108" spans="1:28">
       <c r="A108" s="2" t="s">
         <v>538</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:28" hidden="1">
+    <row r="109" spans="1:28">
       <c r="A109" s="2" t="s">
         <v>539</v>
       </c>
@@ -13032,7 +13032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="1:28" hidden="1">
+    <row r="110" spans="1:28">
       <c r="A110" s="3" t="s">
         <v>986</v>
       </c>
@@ -13108,7 +13108,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="1:28" hidden="1">
+    <row r="111" spans="1:28">
       <c r="A111" s="2" t="s">
         <v>543</v>
       </c>
@@ -13186,7 +13186,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="112" spans="1:28" hidden="1">
+    <row r="112" spans="1:28">
       <c r="A112" s="2" t="s">
         <v>545</v>
       </c>
@@ -13344,7 +13344,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="114" spans="1:28" hidden="1">
+    <row r="114" spans="1:28">
       <c r="A114" s="2" t="s">
         <v>548</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="115" spans="1:28" hidden="1">
+    <row r="115" spans="1:28">
       <c r="A115" s="3" t="s">
         <v>190</v>
       </c>
@@ -13496,7 +13496,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:28" hidden="1">
+    <row r="116" spans="1:28">
       <c r="A116" s="3" t="s">
         <v>1210</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="1:28" hidden="1">
+    <row r="118" spans="1:28">
       <c r="A118" s="2" t="s">
         <v>555</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="119" spans="1:28" hidden="1">
+    <row r="119" spans="1:28">
       <c r="A119" s="2" t="s">
         <v>558</v>
       </c>
@@ -13814,7 +13814,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:28" hidden="1">
+    <row r="120" spans="1:28">
       <c r="A120" s="2" t="s">
         <v>561</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="121" spans="1:28" hidden="1">
+    <row r="121" spans="1:28">
       <c r="A121" s="2" t="s">
         <v>567</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="122" spans="1:28" hidden="1">
+    <row r="122" spans="1:28">
       <c r="A122" s="2" t="s">
         <v>569</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="123" spans="1:28" hidden="1">
+    <row r="123" spans="1:28">
       <c r="A123" s="2" t="s">
         <v>16</v>
       </c>
@@ -14362,7 +14362,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="127" spans="1:28" hidden="1">
+    <row r="127" spans="1:28">
       <c r="A127" s="2" t="s">
         <v>580</v>
       </c>
@@ -14674,7 +14674,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="1:28" hidden="1">
+    <row r="131" spans="1:28">
       <c r="A131" s="2" t="s">
         <v>591</v>
       </c>
@@ -14756,7 +14756,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="132" spans="1:28" hidden="1">
+    <row r="132" spans="1:28">
       <c r="A132" s="2" t="s">
         <v>595</v>
       </c>
@@ -14838,7 +14838,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="133" spans="1:28" hidden="1">
+    <row r="133" spans="1:28">
       <c r="A133" s="2" t="s">
         <v>617</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="134" spans="1:28" hidden="1">
+    <row r="134" spans="1:28">
       <c r="A134" s="2" t="s">
         <v>621</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="135" spans="1:28" hidden="1">
+    <row r="135" spans="1:28">
       <c r="A135" s="2" t="s">
         <v>625</v>
       </c>
@@ -15078,7 +15078,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="136" spans="1:28" hidden="1">
+    <row r="136" spans="1:28">
       <c r="A136" s="2" t="s">
         <v>628</v>
       </c>
@@ -15156,7 +15156,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="137" spans="1:28" hidden="1">
+    <row r="137" spans="1:28">
       <c r="A137" s="2" t="s">
         <v>632</v>
       </c>
@@ -15234,7 +15234,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="138" spans="1:28" hidden="1">
+    <row r="138" spans="1:28">
       <c r="A138" s="2" t="s">
         <v>637</v>
       </c>
@@ -15628,7 +15628,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="143" spans="1:28" hidden="1">
+    <row r="143" spans="1:28">
       <c r="A143" s="3" t="s">
         <v>827</v>
       </c>
@@ -15702,7 +15702,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:28" hidden="1">
+    <row r="144" spans="1:28">
       <c r="A144" s="2" t="s">
         <v>646</v>
       </c>
@@ -15782,7 +15782,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" spans="1:28" s="18" customFormat="1" hidden="1">
+    <row r="145" spans="1:28" s="18" customFormat="1">
       <c r="A145" s="2" t="s">
         <v>649</v>
       </c>
@@ -15860,7 +15860,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="146" spans="1:28" hidden="1">
+    <row r="146" spans="1:28">
       <c r="A146" s="2" t="s">
         <v>652</v>
       </c>
@@ -15944,7 +15944,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="147" spans="1:28" hidden="1">
+    <row r="147" spans="1:28">
       <c r="A147" s="2" t="s">
         <v>654</v>
       </c>
@@ -16022,7 +16022,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:28" hidden="1">
+    <row r="148" spans="1:28">
       <c r="A148" s="3" t="s">
         <v>1068</v>
       </c>
@@ -16096,7 +16096,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:28" hidden="1">
+    <row r="149" spans="1:28">
       <c r="A149" s="2" t="s">
         <v>658</v>
       </c>
@@ -16178,7 +16178,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:28" hidden="1">
+    <row r="150" spans="1:28">
       <c r="A150" s="2" t="s">
         <v>666</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="151" spans="1:28" hidden="1">
+    <row r="151" spans="1:28">
       <c r="A151" s="2" t="s">
         <v>668</v>
       </c>
@@ -16340,7 +16340,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="152" spans="1:28" hidden="1">
+    <row r="152" spans="1:28">
       <c r="A152" s="2" t="s">
         <v>670</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="153" spans="1:28" hidden="1">
+    <row r="153" spans="1:28">
       <c r="A153" s="3" t="s">
         <v>783</v>
       </c>
@@ -16576,7 +16576,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:28" hidden="1">
+    <row r="155" spans="1:28">
       <c r="A155" s="2" t="s">
         <v>676</v>
       </c>
@@ -16730,7 +16730,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="157" spans="1:28" hidden="1">
+    <row r="157" spans="1:28">
       <c r="A157" s="2" t="s">
         <v>680</v>
       </c>
@@ -16808,7 +16808,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:28" hidden="1">
+    <row r="158" spans="1:28">
       <c r="A158" s="2" t="s">
         <v>682</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:28" hidden="1">
+    <row r="159" spans="1:28">
       <c r="A159" s="2" t="s">
         <v>684</v>
       </c>
@@ -16968,7 +16968,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:28" hidden="1">
+    <row r="160" spans="1:28">
       <c r="A160" s="2" t="s">
         <v>689</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:28" hidden="1">
+    <row r="161" spans="1:28">
       <c r="A161" s="2" t="s">
         <v>691</v>
       </c>
@@ -17122,7 +17122,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="162" spans="1:28" hidden="1">
+    <row r="162" spans="1:28">
       <c r="A162" s="2" t="s">
         <v>894</v>
       </c>
@@ -17200,7 +17200,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="163" spans="1:28" hidden="1">
+    <row r="163" spans="1:28">
       <c r="A163" s="2" t="s">
         <v>696</v>
       </c>
@@ -17280,7 +17280,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="164" spans="1:28" hidden="1">
+    <row r="164" spans="1:28">
       <c r="A164" s="2" t="s">
         <v>1169</v>
       </c>
@@ -17354,7 +17354,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="165" spans="1:28" hidden="1">
+    <row r="165" spans="1:28">
       <c r="A165" s="2" t="s">
         <v>893</v>
       </c>
@@ -17516,7 +17516,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="167" spans="1:28" hidden="1">
+    <row r="167" spans="1:28">
       <c r="A167" s="2" t="s">
         <v>706</v>
       </c>
@@ -17598,7 +17598,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:28" hidden="1">
+    <row r="168" spans="1:28">
       <c r="A168" s="2" t="s">
         <v>709</v>
       </c>
@@ -17682,7 +17682,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="169" spans="1:28" hidden="1">
+    <row r="169" spans="1:28">
       <c r="A169" s="2" t="s">
         <v>892</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="170" spans="1:28" hidden="1">
+    <row r="170" spans="1:28">
       <c r="A170" s="2" t="s">
         <v>715</v>
       </c>
@@ -17912,7 +17912,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="172" spans="1:28" hidden="1">
+    <row r="172" spans="1:28">
       <c r="A172" s="3" t="s">
         <v>909</v>
       </c>
@@ -18068,7 +18068,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="174" spans="1:28" hidden="1">
+    <row r="174" spans="1:28">
       <c r="A174" s="3" t="s">
         <v>110</v>
       </c>
@@ -18144,7 +18144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="175" spans="1:28" hidden="1">
+    <row r="175" spans="1:28">
       <c r="A175" s="2" t="s">
         <v>722</v>
       </c>
@@ -18222,7 +18222,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="176" spans="1:28" hidden="1">
+    <row r="176" spans="1:28">
       <c r="A176" s="2" t="s">
         <v>763</v>
       </c>
@@ -18378,7 +18378,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="178" spans="1:28" hidden="1">
+    <row r="178" spans="1:28">
       <c r="A178" s="3" t="s">
         <v>1147</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="179" spans="1:28" hidden="1">
+    <row r="179" spans="1:28">
       <c r="A179" s="2" t="s">
         <v>725</v>
       </c>
@@ -18534,7 +18534,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="180" spans="1:28" hidden="1">
+    <row r="180" spans="1:28">
       <c r="A180" s="2" t="s">
         <v>730</v>
       </c>
@@ -18616,7 +18616,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="181" spans="1:28" hidden="1">
+    <row r="181" spans="1:28">
       <c r="A181" s="2" t="s">
         <v>732</v>
       </c>
@@ -18780,7 +18780,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="183" spans="1:28" hidden="1">
+    <row r="183" spans="1:28">
       <c r="A183" s="2" t="s">
         <v>739</v>
       </c>
@@ -19174,7 +19174,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="188" spans="1:28" hidden="1">
+    <row r="188" spans="1:28">
       <c r="A188" s="2" t="s">
         <v>5</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="189" spans="1:28" hidden="1">
+    <row r="189" spans="1:28">
       <c r="A189" s="3" t="s">
         <v>1103</v>
       </c>
@@ -19334,7 +19334,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="190" spans="1:28" hidden="1">
+    <row r="190" spans="1:28">
       <c r="A190" s="2" t="s">
         <v>776</v>
       </c>
@@ -19416,7 +19416,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="191" spans="1:28" hidden="1">
+    <row r="191" spans="1:28">
       <c r="A191" s="2" t="s">
         <v>809</v>
       </c>
@@ -19498,7 +19498,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="192" spans="1:28" hidden="1">
+    <row r="192" spans="1:28">
       <c r="A192" s="2" t="s">
         <v>813</v>
       </c>
@@ -19576,7 +19576,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="193" spans="1:28" hidden="1">
+    <row r="193" spans="1:28">
       <c r="A193" s="2" t="s">
         <v>815</v>
       </c>
@@ -19660,7 +19660,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="194" spans="1:28" hidden="1">
+    <row r="194" spans="1:28">
       <c r="A194" s="2" t="s">
         <v>1111</v>
       </c>
@@ -19738,7 +19738,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="195" spans="1:28" hidden="1">
+    <row r="195" spans="1:28">
       <c r="A195" s="2" t="s">
         <v>817</v>
       </c>
@@ -19820,7 +19820,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="196" spans="1:28" hidden="1">
+    <row r="196" spans="1:28">
       <c r="A196" s="2" t="s">
         <v>820</v>
       </c>
@@ -19898,7 +19898,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="197" spans="1:28" hidden="1">
+    <row r="197" spans="1:28">
       <c r="A197" s="2" t="s">
         <v>822</v>
       </c>
@@ -19982,7 +19982,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="198" spans="1:28" hidden="1">
+    <row r="198" spans="1:28">
       <c r="A198" s="2" t="s">
         <v>834</v>
       </c>
@@ -20060,7 +20060,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:28" hidden="1">
+    <row r="199" spans="1:28">
       <c r="A199" s="2" t="s">
         <v>835</v>
       </c>
@@ -20140,7 +20140,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="200" spans="1:28" hidden="1">
+    <row r="200" spans="1:28">
       <c r="A200" s="2" t="s">
         <v>837</v>
       </c>
@@ -20220,7 +20220,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="201" spans="1:28" hidden="1">
+    <row r="201" spans="1:28">
       <c r="A201" s="2" t="s">
         <v>843</v>
       </c>
@@ -20300,7 +20300,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="202" spans="1:28" hidden="1">
+    <row r="202" spans="1:28">
       <c r="A202" s="2" t="s">
         <v>853</v>
       </c>
@@ -20384,7 +20384,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="203" spans="1:28" hidden="1">
+    <row r="203" spans="1:28">
       <c r="A203" s="2" t="s">
         <v>857</v>
       </c>
@@ -20546,7 +20546,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="205" spans="1:28" hidden="1">
+    <row r="205" spans="1:28">
       <c r="A205" s="2" t="s">
         <v>409</v>
       </c>
@@ -20628,7 +20628,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="206" spans="1:28" hidden="1">
+    <row r="206" spans="1:28">
       <c r="A206" s="2" t="s">
         <v>411</v>
       </c>
@@ -20708,7 +20708,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="207" spans="1:28" hidden="1">
+    <row r="207" spans="1:28">
       <c r="A207" s="2" t="s">
         <v>414</v>
       </c>
@@ -20786,7 +20786,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="208" spans="1:28" hidden="1">
+    <row r="208" spans="1:28">
       <c r="A208" s="2" t="s">
         <v>415</v>
       </c>
@@ -20866,7 +20866,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="209" spans="1:28" hidden="1">
+    <row r="209" spans="1:28">
       <c r="A209" s="2" t="s">
         <v>419</v>
       </c>
@@ -20950,7 +20950,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="210" spans="1:28" hidden="1">
+    <row r="210" spans="1:28">
       <c r="A210" s="2" t="s">
         <v>424</v>
       </c>
@@ -21028,7 +21028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="211" spans="1:28" hidden="1">
+    <row r="211" spans="1:28">
       <c r="A211" s="3" t="s">
         <v>103</v>
       </c>
@@ -21100,7 +21100,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="212" spans="1:28" hidden="1">
+    <row r="212" spans="1:28">
       <c r="A212" s="2" t="s">
         <v>426</v>
       </c>
@@ -21180,7 +21180,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="213" spans="1:28" hidden="1">
+    <row r="213" spans="1:28">
       <c r="A213" s="3" t="s">
         <v>104</v>
       </c>
@@ -21252,7 +21252,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="214" spans="1:28" hidden="1">
+    <row r="214" spans="1:28">
       <c r="A214" s="2" t="s">
         <v>430</v>
       </c>
@@ -21330,7 +21330,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="215" spans="1:28" hidden="1">
+    <row r="215" spans="1:28">
       <c r="A215" s="3" t="s">
         <v>910</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="217" spans="1:28" hidden="1">
+    <row r="217" spans="1:28">
       <c r="A217" s="2" t="s">
         <v>437</v>
       </c>
@@ -21570,7 +21570,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="218" spans="1:28" hidden="1">
+    <row r="218" spans="1:28">
       <c r="A218" s="3" t="s">
         <v>861</v>
       </c>
@@ -21644,7 +21644,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="219" spans="1:28" hidden="1">
+    <row r="219" spans="1:28">
       <c r="A219" s="2" t="s">
         <v>438</v>
       </c>
@@ -21726,7 +21726,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="220" spans="1:28" hidden="1">
+    <row r="220" spans="1:28">
       <c r="A220" s="2" t="s">
         <v>441</v>
       </c>
@@ -21804,7 +21804,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="221" spans="1:28" hidden="1">
+    <row r="221" spans="1:28">
       <c r="A221" s="2" t="s">
         <v>443</v>
       </c>
@@ -21964,7 +21964,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="223" spans="1:28" hidden="1">
+    <row r="223" spans="1:28">
       <c r="A223" s="2" t="s">
         <v>474</v>
       </c>
@@ -22042,7 +22042,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="224" spans="1:28" hidden="1">
+    <row r="224" spans="1:28">
       <c r="A224" s="2" t="s">
         <v>476</v>
       </c>
@@ -22124,7 +22124,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="225" spans="1:28" hidden="1">
+    <row r="225" spans="1:28">
       <c r="A225" s="2" t="s">
         <v>478</v>
       </c>
@@ -22202,7 +22202,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="226" spans="1:28" hidden="1">
+    <row r="226" spans="1:28">
       <c r="A226" s="35" t="s">
         <v>480</v>
       </c>
@@ -22283,16 +22283,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC226" xr:uid="{C9047C10-536C-FE4C-8D8B-83493895DF5D}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Coal_NI"/>
-        <filter val="Diesel"/>
-        <filter val="Gas"/>
-        <filter val="Geothermal"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC226" xr:uid="{C9047C10-536C-FE4C-8D8B-83493895DF5D}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.17" right="0.22" top="0.66" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="8" scale="74" fitToHeight="0" orientation="portrait"/>
@@ -22304,8 +22295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AFF16F-1931-E143-83E4-C14B2C93AD8E}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
working on profile data strategy pattern
</commit_message>
<xml_diff>
--- a/lib/assets/20151030_Existing_generating_plant.xlsx
+++ b/lib/assets/20151030_Existing_generating_plant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevetorrens/workspace-ror/ghgemissions/lib/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8431F18C-62C1-6A43-9ABE-CCF73846350E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D05D3A-36DD-1F4A-BF53-2AD2E4A7AECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4390,16 +4390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AB226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J63" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4520,7 +4520,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" hidden="1">
       <c r="A2" s="2" t="s">
         <v>326</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" hidden="1">
       <c r="A3" s="2" t="s">
         <v>342</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" hidden="1">
       <c r="A4" s="2" t="s">
         <v>1175</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" hidden="1">
       <c r="A5" s="2" t="s">
         <v>346</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" hidden="1">
       <c r="A6" s="2" t="s">
         <v>353</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" hidden="1">
       <c r="A7" s="2" t="s">
         <v>363</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" hidden="1">
       <c r="A8" s="2" t="s">
         <v>922</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" hidden="1">
       <c r="A9" s="2" t="s">
         <v>926</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" hidden="1">
       <c r="A10" s="2" t="s">
         <v>934</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" hidden="1">
       <c r="A11" s="3" t="s">
         <v>612</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" hidden="1">
       <c r="A12" s="2" t="s">
         <v>940</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" hidden="1">
       <c r="A13" s="2" t="s">
         <v>943</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" hidden="1">
       <c r="A14" s="2" t="s">
         <v>952</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" hidden="1">
       <c r="A15" s="2" t="s">
         <v>960</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" hidden="1">
       <c r="A16" s="2" t="s">
         <v>964</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" hidden="1">
       <c r="A17" s="3" t="s">
         <v>188</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" hidden="1">
       <c r="A18" s="2" t="s">
         <v>970</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" hidden="1">
       <c r="A19" s="2" t="s">
         <v>974</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" hidden="1">
       <c r="A20" s="2" t="s">
         <v>754</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" hidden="1">
       <c r="A21" s="2" t="s">
         <v>980</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" hidden="1">
       <c r="A22" s="2" t="s">
         <v>985</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" hidden="1">
       <c r="A23" s="3" t="s">
         <v>862</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" hidden="1">
       <c r="A24" s="2" t="s">
         <v>990</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" hidden="1">
       <c r="A25" s="2" t="s">
         <v>995</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" hidden="1">
       <c r="A26" s="2" t="s">
         <v>1001</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" hidden="1">
       <c r="A27" s="3" t="s">
         <v>1006</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" hidden="1">
       <c r="A28" s="3" t="s">
         <v>872</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="13" customHeight="1">
+    <row r="29" spans="1:28" ht="13" hidden="1" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>599</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" hidden="1">
       <c r="A30" s="2" t="s">
         <v>1010</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" hidden="1">
       <c r="A31" s="2" t="s">
         <v>1016</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" hidden="1">
       <c r="A32" s="2" t="s">
         <v>1025</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" hidden="1">
       <c r="A33" s="2" t="s">
         <v>1030</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="18" customFormat="1">
+    <row r="34" spans="1:28" s="18" customFormat="1" hidden="1">
       <c r="A34" s="2" t="s">
         <v>1031</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" hidden="1">
       <c r="A35" s="3" t="s">
         <v>510</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" hidden="1">
       <c r="A36" s="2" t="s">
         <v>1036</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" hidden="1">
       <c r="A37" s="2" t="s">
         <v>1041</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" hidden="1">
       <c r="A38" s="2" t="s">
         <v>1045</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" hidden="1">
       <c r="A39" s="3" t="s">
         <v>831</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" hidden="1">
       <c r="A40" s="3" t="s">
         <v>1191</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" hidden="1">
       <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="34" customFormat="1">
+    <row r="42" spans="1:28" s="34" customFormat="1" hidden="1">
       <c r="A42" s="29" t="s">
         <v>1216</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" hidden="1">
       <c r="A43" s="2" t="s">
         <v>1049</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" hidden="1">
       <c r="A44" s="2" t="s">
         <v>760</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" hidden="1">
       <c r="A45" s="2" t="s">
         <v>1050</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:28" hidden="1">
       <c r="A46" s="2" t="s">
         <v>1051</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" hidden="1">
       <c r="A47" s="2" t="s">
         <v>1053</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:28" hidden="1">
       <c r="A48" s="2" t="s">
         <v>1058</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="49" spans="1:28">
+    <row r="49" spans="1:28" hidden="1">
       <c r="A49" s="2" t="s">
         <v>1062</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="1:28">
+    <row r="50" spans="1:28" hidden="1">
       <c r="A50" s="3" t="s">
         <v>794</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="1:28">
+    <row r="51" spans="1:28" hidden="1">
       <c r="A51" s="2" t="s">
         <v>1070</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:28">
+    <row r="52" spans="1:28" hidden="1">
       <c r="A52" s="3" t="s">
         <v>885</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:28">
+    <row r="53" spans="1:28" hidden="1">
       <c r="A53" s="2" t="s">
         <v>1076</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" hidden="1">
       <c r="A54" s="2" t="s">
         <v>43</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" hidden="1">
       <c r="A55" s="2" t="s">
         <v>49</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:28">
+    <row r="56" spans="1:28" hidden="1">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:28">
+    <row r="57" spans="1:28" hidden="1">
       <c r="A57" s="2" t="s">
         <v>63</v>
       </c>
@@ -8936,7 +8936,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="58" spans="1:28">
+    <row r="58" spans="1:28" hidden="1">
       <c r="A58" s="3" t="s">
         <v>798</v>
       </c>
@@ -9012,7 +9012,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="59" spans="1:28">
+    <row r="59" spans="1:28" hidden="1">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="60" spans="1:28">
+    <row r="60" spans="1:28" hidden="1">
       <c r="A60" s="3" t="s">
         <v>895</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:28">
+    <row r="61" spans="1:28" hidden="1">
       <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
@@ -9246,7 +9246,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="62" spans="1:28">
+    <row r="62" spans="1:28" hidden="1">
       <c r="A62" s="3" t="s">
         <v>875</v>
       </c>
@@ -9406,7 +9406,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="1:28">
+    <row r="64" spans="1:28" hidden="1">
       <c r="A64" s="2" t="s">
         <v>85</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="1:28">
+    <row r="65" spans="1:28" hidden="1">
       <c r="A65" s="2" t="s">
         <v>89</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" hidden="1">
       <c r="A66" s="3" t="s">
         <v>759</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="67" spans="1:28">
+    <row r="67" spans="1:28" hidden="1">
       <c r="A67" s="2" t="s">
         <v>93</v>
       </c>
@@ -9716,7 +9716,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="68" spans="1:28">
+    <row r="68" spans="1:28" hidden="1">
       <c r="A68" s="3" t="s">
         <v>787</v>
       </c>
@@ -9792,7 +9792,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="69" spans="1:28">
+    <row r="69" spans="1:28" hidden="1">
       <c r="A69" s="2" t="s">
         <v>94</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="70" spans="1:28">
+    <row r="70" spans="1:28" hidden="1">
       <c r="A70" s="2" t="s">
         <v>98</v>
       </c>
@@ -9958,7 +9958,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:28">
+    <row r="71" spans="1:28" hidden="1">
       <c r="A71" s="2" t="s">
         <v>126</v>
       </c>
@@ -10038,7 +10038,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:28">
+    <row r="72" spans="1:28" hidden="1">
       <c r="A72" s="2" t="s">
         <v>131</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="73" spans="1:28">
+    <row r="73" spans="1:28" hidden="1">
       <c r="A73" s="2" t="s">
         <v>137</v>
       </c>
@@ -10202,7 +10202,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="74" spans="1:28">
+    <row r="74" spans="1:28" hidden="1">
       <c r="A74" s="2" t="s">
         <v>141</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:28">
+    <row r="75" spans="1:28" hidden="1">
       <c r="A75" s="3" t="s">
         <v>662</v>
       </c>
@@ -10356,7 +10356,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="76" spans="1:28">
+    <row r="76" spans="1:28" hidden="1">
       <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
@@ -10428,7 +10428,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="34" customFormat="1">
+    <row r="77" spans="1:28" s="34" customFormat="1" hidden="1">
       <c r="A77" s="30" t="s">
         <v>32</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:28">
+    <row r="78" spans="1:28" hidden="1">
       <c r="A78" s="2" t="s">
         <v>244</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:28">
+    <row r="79" spans="1:28" hidden="1">
       <c r="A79" s="3" t="s">
         <v>112</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:28">
+    <row r="80" spans="1:28" hidden="1">
       <c r="A80" s="2" t="s">
         <v>249</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:28">
+    <row r="81" spans="1:28" hidden="1">
       <c r="A81" s="2" t="s">
         <v>252</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="82" spans="1:28">
+    <row r="82" spans="1:28" hidden="1">
       <c r="A82" s="2" t="s">
         <v>255</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:28">
+    <row r="83" spans="1:28" hidden="1">
       <c r="A83" s="3" t="s">
         <v>800</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="84" spans="1:28">
+    <row r="84" spans="1:28" hidden="1">
       <c r="A84" s="2" t="s">
         <v>296</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" hidden="1">
       <c r="A85" s="3" t="s">
         <v>881</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:28">
+    <row r="86" spans="1:28" hidden="1">
       <c r="A86" s="2" t="s">
         <v>481</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="87" spans="1:28">
+    <row r="87" spans="1:28" hidden="1">
       <c r="A87" s="2" t="s">
         <v>482</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="34" customFormat="1">
+    <row r="88" spans="1:28" s="34" customFormat="1" hidden="1">
       <c r="A88" s="29" t="s">
         <v>1217</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:28">
+    <row r="89" spans="1:28" hidden="1">
       <c r="A89" s="2" t="s">
         <v>489</v>
       </c>
@@ -11456,7 +11456,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="90" spans="1:28">
+    <row r="90" spans="1:28" hidden="1">
       <c r="A90" s="2" t="s">
         <v>492</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="91" spans="1:28">
+    <row r="91" spans="1:28" hidden="1">
       <c r="A91" s="3" t="s">
         <v>901</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:28">
+    <row r="92" spans="1:28" hidden="1">
       <c r="A92" s="3" t="s">
         <v>269</v>
       </c>
@@ -11692,7 +11692,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" hidden="1">
       <c r="A93" s="2" t="s">
         <v>495</v>
       </c>
@@ -11772,7 +11772,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:28">
+    <row r="94" spans="1:28" hidden="1">
       <c r="A94" s="2" t="s">
         <v>501</v>
       </c>
@@ -11854,7 +11854,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:28">
+    <row r="95" spans="1:28" hidden="1">
       <c r="A95" s="2" t="s">
         <v>79</v>
       </c>
@@ -11926,7 +11926,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:28">
+    <row r="96" spans="1:28" hidden="1">
       <c r="A96" s="2" t="s">
         <v>506</v>
       </c>
@@ -12006,7 +12006,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="97" spans="1:28">
+    <row r="97" spans="1:28" hidden="1">
       <c r="A97" s="2" t="s">
         <v>508</v>
       </c>
@@ -12084,7 +12084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:28">
+    <row r="98" spans="1:28" hidden="1">
       <c r="A98" s="2" t="s">
         <v>513</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="1:28">
+    <row r="99" spans="1:28" hidden="1">
       <c r="A99" s="2" t="s">
         <v>515</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:28">
+    <row r="100" spans="1:28" hidden="1">
       <c r="A100" s="2" t="s">
         <v>519</v>
       </c>
@@ -12322,7 +12322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:28">
+    <row r="101" spans="1:28" hidden="1">
       <c r="A101" s="2" t="s">
         <v>521</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="102" spans="1:28">
+    <row r="102" spans="1:28" hidden="1">
       <c r="A102" s="2" t="s">
         <v>58</v>
       </c>
@@ -12482,7 +12482,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="103" spans="1:28">
+    <row r="103" spans="1:28" hidden="1">
       <c r="A103" s="2" t="s">
         <v>805</v>
       </c>
@@ -12560,7 +12560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:28">
+    <row r="104" spans="1:28" hidden="1">
       <c r="A104" s="3" t="s">
         <v>806</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="105" spans="1:28">
+    <row r="105" spans="1:28" hidden="1">
       <c r="A105" s="2" t="s">
         <v>531</v>
       </c>
@@ -12714,7 +12714,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="106" spans="1:28">
+    <row r="106" spans="1:28" hidden="1">
       <c r="A106" s="2" t="s">
         <v>533</v>
       </c>
@@ -12794,7 +12794,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="107" spans="1:28">
+    <row r="107" spans="1:28" hidden="1">
       <c r="A107" s="3" t="s">
         <v>2</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:28">
+    <row r="108" spans="1:28" hidden="1">
       <c r="A108" s="2" t="s">
         <v>538</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:28" hidden="1">
       <c r="A109" s="2" t="s">
         <v>539</v>
       </c>
@@ -13032,7 +13032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:28" hidden="1">
       <c r="A110" s="3" t="s">
         <v>986</v>
       </c>
@@ -13108,7 +13108,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="1:28">
+    <row r="111" spans="1:28" hidden="1">
       <c r="A111" s="2" t="s">
         <v>543</v>
       </c>
@@ -13186,7 +13186,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="112" spans="1:28">
+    <row r="112" spans="1:28" hidden="1">
       <c r="A112" s="2" t="s">
         <v>545</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:28">
+    <row r="113" spans="1:28" hidden="1">
       <c r="A113" s="2" t="s">
         <v>1180</v>
       </c>
@@ -13344,7 +13344,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="114" spans="1:28">
+    <row r="114" spans="1:28" hidden="1">
       <c r="A114" s="2" t="s">
         <v>548</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="115" spans="1:28">
+    <row r="115" spans="1:28" hidden="1">
       <c r="A115" s="3" t="s">
         <v>190</v>
       </c>
@@ -13496,7 +13496,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:28">
+    <row r="116" spans="1:28" hidden="1">
       <c r="A116" s="3" t="s">
         <v>1210</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:28">
+    <row r="117" spans="1:28" hidden="1">
       <c r="A117" s="2" t="s">
         <v>517</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="1:28">
+    <row r="118" spans="1:28" hidden="1">
       <c r="A118" s="2" t="s">
         <v>555</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="119" spans="1:28">
+    <row r="119" spans="1:28" hidden="1">
       <c r="A119" s="2" t="s">
         <v>558</v>
       </c>
@@ -13814,7 +13814,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:28">
+    <row r="120" spans="1:28" hidden="1">
       <c r="A120" s="2" t="s">
         <v>561</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="121" spans="1:28">
+    <row r="121" spans="1:28" hidden="1">
       <c r="A121" s="2" t="s">
         <v>567</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="122" spans="1:28">
+    <row r="122" spans="1:28" hidden="1">
       <c r="A122" s="2" t="s">
         <v>569</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="123" spans="1:28">
+    <row r="123" spans="1:28" hidden="1">
       <c r="A123" s="2" t="s">
         <v>16</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="124" spans="1:28">
+    <row r="124" spans="1:28" hidden="1">
       <c r="A124" s="3" t="s">
         <v>913</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="125" spans="1:28">
+    <row r="125" spans="1:28" hidden="1">
       <c r="A125" s="2" t="s">
         <v>574</v>
       </c>
@@ -14284,7 +14284,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="1:28">
+    <row r="126" spans="1:28" hidden="1">
       <c r="A126" s="3" t="s">
         <v>261</v>
       </c>
@@ -14362,7 +14362,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="127" spans="1:28">
+    <row r="127" spans="1:28" hidden="1">
       <c r="A127" s="2" t="s">
         <v>580</v>
       </c>
@@ -14438,7 +14438,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="128" spans="1:28">
+    <row r="128" spans="1:28" hidden="1">
       <c r="A128" s="2" t="s">
         <v>26</v>
       </c>
@@ -14514,7 +14514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:28">
+    <row r="129" spans="1:28" hidden="1">
       <c r="A129" s="16" t="s">
         <v>582</v>
       </c>
@@ -14594,7 +14594,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="1:28">
+    <row r="130" spans="1:28" hidden="1">
       <c r="A130" s="2" t="s">
         <v>587</v>
       </c>
@@ -14674,7 +14674,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="1:28">
+    <row r="131" spans="1:28" hidden="1">
       <c r="A131" s="2" t="s">
         <v>591</v>
       </c>
@@ -14756,7 +14756,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="132" spans="1:28">
+    <row r="132" spans="1:28" hidden="1">
       <c r="A132" s="2" t="s">
         <v>595</v>
       </c>
@@ -14838,7 +14838,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="133" spans="1:28">
+    <row r="133" spans="1:28" hidden="1">
       <c r="A133" s="2" t="s">
         <v>617</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="134" spans="1:28">
+    <row r="134" spans="1:28" hidden="1">
       <c r="A134" s="2" t="s">
         <v>621</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="135" spans="1:28">
+    <row r="135" spans="1:28" hidden="1">
       <c r="A135" s="2" t="s">
         <v>625</v>
       </c>
@@ -15078,7 +15078,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="136" spans="1:28">
+    <row r="136" spans="1:28" hidden="1">
       <c r="A136" s="2" t="s">
         <v>628</v>
       </c>
@@ -15156,7 +15156,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="137" spans="1:28">
+    <row r="137" spans="1:28" hidden="1">
       <c r="A137" s="2" t="s">
         <v>632</v>
       </c>
@@ -15234,7 +15234,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="138" spans="1:28">
+    <row r="138" spans="1:28" hidden="1">
       <c r="A138" s="2" t="s">
         <v>637</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="139" spans="1:28">
+    <row r="139" spans="1:28" hidden="1">
       <c r="A139" s="2" t="s">
         <v>796</v>
       </c>
@@ -15390,7 +15390,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:28">
+    <row r="140" spans="1:28" hidden="1">
       <c r="A140" s="2" t="s">
         <v>797</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:28">
+    <row r="141" spans="1:28" hidden="1">
       <c r="A141" s="2" t="s">
         <v>639</v>
       </c>
@@ -15548,7 +15548,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="142" spans="1:28">
+    <row r="142" spans="1:28" hidden="1">
       <c r="A142" s="2" t="s">
         <v>642</v>
       </c>
@@ -15628,7 +15628,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="143" spans="1:28">
+    <row r="143" spans="1:28" hidden="1">
       <c r="A143" s="3" t="s">
         <v>827</v>
       </c>
@@ -15702,7 +15702,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:28">
+    <row r="144" spans="1:28" hidden="1">
       <c r="A144" s="2" t="s">
         <v>646</v>
       </c>
@@ -15782,7 +15782,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" spans="1:28" s="18" customFormat="1">
+    <row r="145" spans="1:28" s="18" customFormat="1" hidden="1">
       <c r="A145" s="2" t="s">
         <v>649</v>
       </c>
@@ -15860,7 +15860,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="146" spans="1:28">
+    <row r="146" spans="1:28" hidden="1">
       <c r="A146" s="2" t="s">
         <v>652</v>
       </c>
@@ -15944,7 +15944,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="147" spans="1:28">
+    <row r="147" spans="1:28" hidden="1">
       <c r="A147" s="2" t="s">
         <v>654</v>
       </c>
@@ -16022,7 +16022,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:28">
+    <row r="148" spans="1:28" hidden="1">
       <c r="A148" s="3" t="s">
         <v>1068</v>
       </c>
@@ -16096,7 +16096,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:28">
+    <row r="149" spans="1:28" hidden="1">
       <c r="A149" s="2" t="s">
         <v>658</v>
       </c>
@@ -16178,7 +16178,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:28">
+    <row r="150" spans="1:28" hidden="1">
       <c r="A150" s="2" t="s">
         <v>666</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="151" spans="1:28">
+    <row r="151" spans="1:28" hidden="1">
       <c r="A151" s="2" t="s">
         <v>668</v>
       </c>
@@ -16340,7 +16340,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="152" spans="1:28">
+    <row r="152" spans="1:28" hidden="1">
       <c r="A152" s="2" t="s">
         <v>670</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="153" spans="1:28">
+    <row r="153" spans="1:28" hidden="1">
       <c r="A153" s="3" t="s">
         <v>783</v>
       </c>
@@ -16496,7 +16496,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="154" spans="1:28">
+    <row r="154" spans="1:28" hidden="1">
       <c r="A154" s="3" t="s">
         <v>673</v>
       </c>
@@ -16576,7 +16576,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:28">
+    <row r="155" spans="1:28" hidden="1">
       <c r="A155" s="2" t="s">
         <v>676</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="156" spans="1:28">
+    <row r="156" spans="1:28" hidden="1">
       <c r="A156" s="2" t="s">
         <v>608</v>
       </c>
@@ -16730,7 +16730,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="157" spans="1:28">
+    <row r="157" spans="1:28" hidden="1">
       <c r="A157" s="2" t="s">
         <v>680</v>
       </c>
@@ -16808,7 +16808,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:28">
+    <row r="158" spans="1:28" hidden="1">
       <c r="A158" s="2" t="s">
         <v>682</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:28">
+    <row r="159" spans="1:28" hidden="1">
       <c r="A159" s="2" t="s">
         <v>684</v>
       </c>
@@ -16968,7 +16968,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:28">
+    <row r="160" spans="1:28" hidden="1">
       <c r="A160" s="2" t="s">
         <v>689</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:28">
+    <row r="161" spans="1:28" hidden="1">
       <c r="A161" s="2" t="s">
         <v>691</v>
       </c>
@@ -17122,7 +17122,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="162" spans="1:28">
+    <row r="162" spans="1:28" hidden="1">
       <c r="A162" s="2" t="s">
         <v>894</v>
       </c>
@@ -17200,7 +17200,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="163" spans="1:28">
+    <row r="163" spans="1:28" hidden="1">
       <c r="A163" s="2" t="s">
         <v>696</v>
       </c>
@@ -17280,7 +17280,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="164" spans="1:28">
+    <row r="164" spans="1:28" hidden="1">
       <c r="A164" s="2" t="s">
         <v>1169</v>
       </c>
@@ -17354,7 +17354,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="165" spans="1:28">
+    <row r="165" spans="1:28" hidden="1">
       <c r="A165" s="2" t="s">
         <v>893</v>
       </c>
@@ -17434,7 +17434,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="166" spans="1:28">
+    <row r="166" spans="1:28" hidden="1">
       <c r="A166" s="2" t="s">
         <v>702</v>
       </c>
@@ -17516,7 +17516,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="167" spans="1:28">
+    <row r="167" spans="1:28" hidden="1">
       <c r="A167" s="2" t="s">
         <v>706</v>
       </c>
@@ -17598,7 +17598,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:28">
+    <row r="168" spans="1:28" hidden="1">
       <c r="A168" s="2" t="s">
         <v>709</v>
       </c>
@@ -17682,7 +17682,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="169" spans="1:28">
+    <row r="169" spans="1:28" hidden="1">
       <c r="A169" s="2" t="s">
         <v>892</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="170" spans="1:28">
+    <row r="170" spans="1:28" hidden="1">
       <c r="A170" s="2" t="s">
         <v>715</v>
       </c>
@@ -17840,7 +17840,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="171" spans="1:28">
+    <row r="171" spans="1:28" hidden="1">
       <c r="A171" s="3" t="s">
         <v>790</v>
       </c>
@@ -17912,7 +17912,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="172" spans="1:28">
+    <row r="172" spans="1:28" hidden="1">
       <c r="A172" s="3" t="s">
         <v>909</v>
       </c>
@@ -17986,7 +17986,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="173" spans="1:28" s="34" customFormat="1">
+    <row r="173" spans="1:28" s="34" customFormat="1" hidden="1">
       <c r="A173" s="29" t="s">
         <v>718</v>
       </c>
@@ -18068,7 +18068,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="174" spans="1:28">
+    <row r="174" spans="1:28" hidden="1">
       <c r="A174" s="3" t="s">
         <v>110</v>
       </c>
@@ -18144,7 +18144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="175" spans="1:28">
+    <row r="175" spans="1:28" hidden="1">
       <c r="A175" s="2" t="s">
         <v>722</v>
       </c>
@@ -18222,7 +18222,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="176" spans="1:28">
+    <row r="176" spans="1:28" hidden="1">
       <c r="A176" s="2" t="s">
         <v>763</v>
       </c>
@@ -18300,7 +18300,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="177" spans="1:28">
+    <row r="177" spans="1:28" hidden="1">
       <c r="A177" s="3" t="s">
         <v>1143</v>
       </c>
@@ -18378,7 +18378,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="178" spans="1:28">
+    <row r="178" spans="1:28" hidden="1">
       <c r="A178" s="3" t="s">
         <v>1147</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="179" spans="1:28">
+    <row r="179" spans="1:28" hidden="1">
       <c r="A179" s="2" t="s">
         <v>725</v>
       </c>
@@ -18534,7 +18534,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="180" spans="1:28">
+    <row r="180" spans="1:28" hidden="1">
       <c r="A180" s="2" t="s">
         <v>730</v>
       </c>
@@ -18616,7 +18616,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="181" spans="1:28">
+    <row r="181" spans="1:28" hidden="1">
       <c r="A181" s="2" t="s">
         <v>732</v>
       </c>
@@ -18700,7 +18700,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="182" spans="1:28">
+    <row r="182" spans="1:28" hidden="1">
       <c r="A182" s="2" t="s">
         <v>735</v>
       </c>
@@ -18780,7 +18780,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="183" spans="1:28">
+    <row r="183" spans="1:28" hidden="1">
       <c r="A183" s="2" t="s">
         <v>739</v>
       </c>
@@ -18860,7 +18860,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="184" spans="1:28">
+    <row r="184" spans="1:28" hidden="1">
       <c r="A184" s="2" t="s">
         <v>743</v>
       </c>
@@ -18940,7 +18940,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="185" spans="1:28">
+    <row r="185" spans="1:28" hidden="1">
       <c r="A185" s="3" t="s">
         <v>1106</v>
       </c>
@@ -19016,7 +19016,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="186" spans="1:28">
+    <row r="186" spans="1:28" hidden="1">
       <c r="A186" s="3" t="s">
         <v>1193</v>
       </c>
@@ -19094,7 +19094,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="187" spans="1:28">
+    <row r="187" spans="1:28" hidden="1">
       <c r="A187" s="2" t="s">
         <v>770</v>
       </c>
@@ -19174,7 +19174,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="188" spans="1:28">
+    <row r="188" spans="1:28" hidden="1">
       <c r="A188" s="2" t="s">
         <v>5</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="189" spans="1:28">
+    <row r="189" spans="1:28" hidden="1">
       <c r="A189" s="3" t="s">
         <v>1103</v>
       </c>
@@ -19334,7 +19334,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="190" spans="1:28">
+    <row r="190" spans="1:28" hidden="1">
       <c r="A190" s="2" t="s">
         <v>776</v>
       </c>
@@ -19416,7 +19416,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="191" spans="1:28">
+    <row r="191" spans="1:28" hidden="1">
       <c r="A191" s="2" t="s">
         <v>809</v>
       </c>
@@ -19498,7 +19498,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="192" spans="1:28">
+    <row r="192" spans="1:28" hidden="1">
       <c r="A192" s="2" t="s">
         <v>813</v>
       </c>
@@ -19576,7 +19576,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="193" spans="1:28">
+    <row r="193" spans="1:28" hidden="1">
       <c r="A193" s="2" t="s">
         <v>815</v>
       </c>
@@ -19660,7 +19660,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="194" spans="1:28">
+    <row r="194" spans="1:28" hidden="1">
       <c r="A194" s="2" t="s">
         <v>1111</v>
       </c>
@@ -19738,7 +19738,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="195" spans="1:28">
+    <row r="195" spans="1:28" hidden="1">
       <c r="A195" s="2" t="s">
         <v>817</v>
       </c>
@@ -19820,7 +19820,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="196" spans="1:28">
+    <row r="196" spans="1:28" hidden="1">
       <c r="A196" s="2" t="s">
         <v>820</v>
       </c>
@@ -19898,7 +19898,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="197" spans="1:28">
+    <row r="197" spans="1:28" hidden="1">
       <c r="A197" s="2" t="s">
         <v>822</v>
       </c>
@@ -19982,7 +19982,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="198" spans="1:28">
+    <row r="198" spans="1:28" hidden="1">
       <c r="A198" s="2" t="s">
         <v>834</v>
       </c>
@@ -20060,7 +20060,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:28">
+    <row r="199" spans="1:28" hidden="1">
       <c r="A199" s="2" t="s">
         <v>835</v>
       </c>
@@ -20140,7 +20140,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="200" spans="1:28">
+    <row r="200" spans="1:28" hidden="1">
       <c r="A200" s="2" t="s">
         <v>837</v>
       </c>
@@ -20220,7 +20220,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="201" spans="1:28">
+    <row r="201" spans="1:28" hidden="1">
       <c r="A201" s="2" t="s">
         <v>843</v>
       </c>
@@ -20300,7 +20300,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="202" spans="1:28">
+    <row r="202" spans="1:28" hidden="1">
       <c r="A202" s="2" t="s">
         <v>853</v>
       </c>
@@ -20384,7 +20384,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="203" spans="1:28">
+    <row r="203" spans="1:28" hidden="1">
       <c r="A203" s="2" t="s">
         <v>857</v>
       </c>
@@ -20464,7 +20464,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="204" spans="1:28">
+    <row r="204" spans="1:28" hidden="1">
       <c r="A204" s="2" t="s">
         <v>405</v>
       </c>
@@ -20546,7 +20546,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="205" spans="1:28">
+    <row r="205" spans="1:28" hidden="1">
       <c r="A205" s="2" t="s">
         <v>409</v>
       </c>
@@ -20628,7 +20628,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="206" spans="1:28">
+    <row r="206" spans="1:28" hidden="1">
       <c r="A206" s="2" t="s">
         <v>411</v>
       </c>
@@ -20708,7 +20708,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="207" spans="1:28">
+    <row r="207" spans="1:28" hidden="1">
       <c r="A207" s="2" t="s">
         <v>414</v>
       </c>
@@ -20786,7 +20786,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="208" spans="1:28">
+    <row r="208" spans="1:28" hidden="1">
       <c r="A208" s="2" t="s">
         <v>415</v>
       </c>
@@ -20866,7 +20866,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="209" spans="1:28">
+    <row r="209" spans="1:28" hidden="1">
       <c r="A209" s="2" t="s">
         <v>419</v>
       </c>
@@ -20950,7 +20950,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="210" spans="1:28">
+    <row r="210" spans="1:28" hidden="1">
       <c r="A210" s="2" t="s">
         <v>424</v>
       </c>
@@ -21028,7 +21028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="211" spans="1:28">
+    <row r="211" spans="1:28" hidden="1">
       <c r="A211" s="3" t="s">
         <v>103</v>
       </c>
@@ -21100,7 +21100,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="212" spans="1:28">
+    <row r="212" spans="1:28" hidden="1">
       <c r="A212" s="2" t="s">
         <v>426</v>
       </c>
@@ -21180,7 +21180,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="213" spans="1:28">
+    <row r="213" spans="1:28" hidden="1">
       <c r="A213" s="3" t="s">
         <v>104</v>
       </c>
@@ -21252,7 +21252,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="214" spans="1:28">
+    <row r="214" spans="1:28" hidden="1">
       <c r="A214" s="2" t="s">
         <v>430</v>
       </c>
@@ -21330,7 +21330,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="215" spans="1:28">
+    <row r="215" spans="1:28" hidden="1">
       <c r="A215" s="3" t="s">
         <v>910</v>
       </c>
@@ -21410,7 +21410,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="216" spans="1:28">
+    <row r="216" spans="1:28" hidden="1">
       <c r="A216" s="2" t="s">
         <v>434</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="217" spans="1:28">
+    <row r="217" spans="1:28" hidden="1">
       <c r="A217" s="2" t="s">
         <v>437</v>
       </c>
@@ -21570,7 +21570,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="218" spans="1:28">
+    <row r="218" spans="1:28" hidden="1">
       <c r="A218" s="3" t="s">
         <v>861</v>
       </c>
@@ -21644,7 +21644,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="219" spans="1:28">
+    <row r="219" spans="1:28" hidden="1">
       <c r="A219" s="2" t="s">
         <v>438</v>
       </c>
@@ -21726,7 +21726,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="220" spans="1:28">
+    <row r="220" spans="1:28" hidden="1">
       <c r="A220" s="2" t="s">
         <v>441</v>
       </c>
@@ -21804,7 +21804,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="221" spans="1:28">
+    <row r="221" spans="1:28" hidden="1">
       <c r="A221" s="2" t="s">
         <v>443</v>
       </c>
@@ -21886,7 +21886,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="222" spans="1:28">
+    <row r="222" spans="1:28" hidden="1">
       <c r="A222" s="2" t="s">
         <v>470</v>
       </c>
@@ -21964,7 +21964,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="223" spans="1:28">
+    <row r="223" spans="1:28" hidden="1">
       <c r="A223" s="2" t="s">
         <v>474</v>
       </c>
@@ -22042,7 +22042,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="224" spans="1:28">
+    <row r="224" spans="1:28" hidden="1">
       <c r="A224" s="2" t="s">
         <v>476</v>
       </c>
@@ -22124,7 +22124,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="225" spans="1:28">
+    <row r="225" spans="1:28" hidden="1">
       <c r="A225" s="2" t="s">
         <v>478</v>
       </c>
@@ -22202,7 +22202,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="226" spans="1:28">
+    <row r="226" spans="1:28" hidden="1">
       <c r="A226" s="35" t="s">
         <v>480</v>
       </c>
@@ -22283,7 +22283,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC226" xr:uid="{C9047C10-536C-FE4C-8D8B-83493895DF5D}"/>
+  <autoFilter ref="A1:AC226" xr:uid="{C9047C10-536C-FE4C-8D8B-83493895DF5D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Huntly"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.17" right="0.22" top="0.66" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="8" scale="74" fitToHeight="0" orientation="portrait"/>

</xml_diff>